<commit_message>
[FIX] se arreglar errores en cargar y clonar semestre
</commit_message>
<xml_diff>
--- a/csv/Planilla_de_Cursos_Prim_2019_Fechas.xlsx
+++ b/csv/Planilla_de_Cursos_Prim_2019_Fechas.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="109">
   <si>
     <t xml:space="preserve">Año</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t xml:space="preserve">Patricio Poblete/Nelson Baloian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/102019</t>
   </si>
   <si>
     <t xml:space="preserve">CC3101: Matem. Discretas para la Comp.</t>
@@ -968,17 +965,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:P961"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.13"/>
@@ -1141,8 +1138,8 @@
       <c r="J7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>33</v>
+      <c r="K7" s="17" t="n">
+        <v>43565</v>
       </c>
       <c r="L7" s="18" t="s">
         <v>30</v>
@@ -1159,32 +1156,32 @@
         <v>22</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="18" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="F8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="G8" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="K8" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
@@ -1197,32 +1194,32 @@
         <v>22</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="18" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>43</v>
-      </c>
       <c r="F9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>38</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="K9" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
@@ -1235,35 +1232,35 @@
         <v>22</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="18" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>26</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="K10" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="L10" s="24" t="s">
         <v>50</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>51</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
@@ -1272,35 +1269,35 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>53</v>
       </c>
       <c r="C11" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="27" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="K11" s="27" t="s">
         <v>56</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>57</v>
       </c>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
@@ -1310,41 +1307,41 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>60</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="K12" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="L12" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="M12" s="27" t="s">
         <v>64</v>
-      </c>
-      <c r="M12" s="27" t="s">
-        <v>65</v>
       </c>
       <c r="N12" s="27"/>
       <c r="O12" s="27"/>
@@ -1352,22 +1349,22 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="27" t="s">
         <v>26</v>
@@ -1384,35 +1381,35 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="27" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="F14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>70</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>71</v>
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="27" t="s">
         <v>72</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>73</v>
       </c>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
@@ -1422,19 +1419,19 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="C15" s="34" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="36" t="s">
         <v>26</v>
@@ -1442,13 +1439,13 @@
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="36" t="s">
         <v>76</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="36" t="s">
-        <v>77</v>
       </c>
       <c r="L15" s="36"/>
       <c r="M15" s="37"/>
@@ -1458,22 +1455,22 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="34" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
@@ -1481,16 +1478,16 @@
         <v>27</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L16" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
@@ -1498,35 +1495,35 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="34" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="34" t="s">
         <v>82</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>83</v>
       </c>
       <c r="G17" s="37" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="37"/>
       <c r="I17" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>25</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L17" s="34" t="s">
         <v>30</v>
@@ -1538,35 +1535,35 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="34" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="34" t="s">
         <v>82</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>83</v>
       </c>
       <c r="G18" s="37" t="s">
         <v>31</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J18" s="34" t="s">
         <v>25</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L18" s="34" t="s">
         <v>30</v>
@@ -1578,38 +1575,38 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="34" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="39" t="s">
-        <v>87</v>
-      </c>
       <c r="G19" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="35" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L19" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="34"/>
@@ -1618,35 +1615,35 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>90</v>
       </c>
       <c r="C20" s="44" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="44" t="s">
-        <v>92</v>
-      </c>
       <c r="G20" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H20" s="44"/>
       <c r="I20" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K20" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L20" s="44"/>
       <c r="M20" s="44"/>
@@ -1656,35 +1653,35 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="44" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="45" t="s">
-        <v>87</v>
-      </c>
       <c r="G21" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="44"/>
       <c r="I21" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J21" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K21" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
@@ -1694,22 +1691,22 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="44" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="44" t="s">
         <v>26</v>
@@ -1726,38 +1723,38 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="48" t="s">
         <v>98</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>99</v>
       </c>
       <c r="C23" s="49" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
       <c r="G23" s="48"/>
       <c r="H23" s="48"/>
       <c r="I23" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="J23" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="J23" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="K23" s="51" t="s">
+      <c r="L23" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="L23" s="51" t="s">
+      <c r="M23" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="M23" s="48" t="s">
-        <v>104</v>
-      </c>
       <c r="N23" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O23" s="48" t="s">
         <v>31</v>
@@ -1766,25 +1763,25 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="53" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" s="53" t="s">
-        <v>106</v>
       </c>
       <c r="C24" s="54" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="F24" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="54" t="s">
         <v>108</v>
-      </c>
-      <c r="F24" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="54" t="s">
-        <v>109</v>
       </c>
       <c r="H24" s="57"/>
       <c r="I24" s="56"/>

</xml_diff>